<commit_message>
UI Updates and Upding te URL removed overwrite
</commit_message>
<xml_diff>
--- a/scan-logs.xlsx
+++ b/scan-logs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1090,9 +1090,49 @@
         <v>١:٣٥:٥١ م</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>2025-11-30T11:25:30.596Z</v>
+      </c>
+      <c r="B35" t="str">
+        <v>rousol@testhost.com</v>
+      </c>
+      <c r="C35" t="str">
+        <v>https://dga.gov.sa</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E35" t="str">
+        <v>٣٠‏/١١‏/٢٠٢٥</v>
+      </c>
+      <c r="F35" t="str">
+        <v>٢:٢٥:٣٠ م</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>2025-11-30T11:33:22.258Z</v>
+      </c>
+      <c r="B36" t="str">
+        <v>sara@test.com</v>
+      </c>
+      <c r="C36" t="str">
+        <v>https://www.arabou.edu.sa/</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E36" t="str">
+        <v>٣٠‏/١١‏/٢٠٢٥</v>
+      </c>
+      <c r="F36" t="str">
+        <v>٢:٣٣:٢٢ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F34"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the Export PDF
</commit_message>
<xml_diff>
--- a/scan-logs.xlsx
+++ b/scan-logs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1130,9 +1130,49 @@
         <v>٢:٣٣:٢٢ م</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>2025-11-30T12:31:12.001Z</v>
+      </c>
+      <c r="B37" t="str">
+        <v>rus@h.com</v>
+      </c>
+      <c r="C37" t="str">
+        <v>https://ksu.edu.sa</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E37" t="str">
+        <v>٣٠‏/١١‏/٢٠٢٥</v>
+      </c>
+      <c r="F37" t="str">
+        <v>٣:٣١:١٢ م</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>2025-11-30T12:38:36.960Z</v>
+      </c>
+      <c r="B38" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="C38" t="str">
+        <v>https://ksu.edu.sa</v>
+      </c>
+      <c r="D38" t="str">
+        <v>No</v>
+      </c>
+      <c r="E38" t="str">
+        <v>٣٠‏/١١‏/٢٠٢٥</v>
+      </c>
+      <c r="F38" t="str">
+        <v>٣:٣٨:٣٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F38"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the seearch bar detection
</commit_message>
<xml_diff>
--- a/scan-logs.xlsx
+++ b/scan-logs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1250,9 +1250,89 @@
         <v>١٢:٠٩:٢٧ م</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>2025-12-03T09:52:08.671Z</v>
+      </c>
+      <c r="B43" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="C43" t="str">
+        <v>https://www.mim.gov.sa/ar</v>
+      </c>
+      <c r="D43" t="str">
+        <v>No</v>
+      </c>
+      <c r="E43" t="str">
+        <v>٣‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F43" t="str">
+        <v>١٢:٥٢:٠٨ م</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>2025-12-03T09:58:02.766Z</v>
+      </c>
+      <c r="B44" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="C44" t="str">
+        <v>https://www.mim.gov.sa/ar</v>
+      </c>
+      <c r="D44" t="str">
+        <v>No</v>
+      </c>
+      <c r="E44" t="str">
+        <v>٣‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F44" t="str">
+        <v>١٢:٥٨:٠٢ م</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>2025-12-03T09:58:37.673Z</v>
+      </c>
+      <c r="B45" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="C45" t="str">
+        <v>https://www.mim.gov.sa/ar</v>
+      </c>
+      <c r="D45" t="str">
+        <v>No</v>
+      </c>
+      <c r="E45" t="str">
+        <v>٣‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F45" t="str">
+        <v>١٢:٥٨:٣٧ م</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>2025-12-03T10:00:57.299Z</v>
+      </c>
+      <c r="B46" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="C46" t="str">
+        <v>https://www.mim.gov.sa/ar</v>
+      </c>
+      <c r="D46" t="str">
+        <v>No</v>
+      </c>
+      <c r="E46" t="str">
+        <v>٣‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F46" t="str">
+        <v>١:٠٠:٥٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F46"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates on the Report page
</commit_message>
<xml_diff>
--- a/scan-logs.xlsx
+++ b/scan-logs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1330,9 +1330,409 @@
         <v>١:٠٠:٥٧ م</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>2025-12-09T12:42:49.728Z</v>
+      </c>
+      <c r="B47" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="C47" t="str">
+        <v>https://pnu.edu.sa</v>
+      </c>
+      <c r="D47" t="str">
+        <v>No</v>
+      </c>
+      <c r="E47" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F47" t="str">
+        <v>٣:٤٢:٤٩ م</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>2025-12-09T12:55:50.316Z</v>
+      </c>
+      <c r="B48" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C48" t="str">
+        <v>https://care.med.sa/</v>
+      </c>
+      <c r="D48" t="str">
+        <v>No</v>
+      </c>
+      <c r="E48" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F48" t="str">
+        <v>٣:٥٥:٥٠ م</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>2025-12-09T12:58:11.542Z</v>
+      </c>
+      <c r="B49" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C49" t="str">
+        <v>https://care.med.sa/</v>
+      </c>
+      <c r="D49" t="str">
+        <v>No</v>
+      </c>
+      <c r="E49" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F49" t="str">
+        <v>٣:٥٨:١١ م</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>2025-12-09T13:03:53.508Z</v>
+      </c>
+      <c r="B50" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C50" t="str">
+        <v>https://care.med.sa/</v>
+      </c>
+      <c r="D50" t="str">
+        <v>No</v>
+      </c>
+      <c r="E50" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F50" t="str">
+        <v>٤:٠٣:٥٣ م</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>2025-12-09T13:08:16.699Z</v>
+      </c>
+      <c r="B51" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C51" t="str">
+        <v>https://care.med.sa/</v>
+      </c>
+      <c r="D51" t="str">
+        <v>No</v>
+      </c>
+      <c r="E51" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F51" t="str">
+        <v>٤:٠٨:١٦ م</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>2025-12-09T13:10:51.186Z</v>
+      </c>
+      <c r="B52" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C52" t="str">
+        <v>https://care.med.sa/</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E52" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F52" t="str">
+        <v>٤:١٠:٥١ م</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>2025-12-09T13:12:28.696Z</v>
+      </c>
+      <c r="B53" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C53" t="str">
+        <v>https://care.med.sa/</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E53" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F53" t="str">
+        <v>٤:١٢:٢٨ م</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>2025-12-09T13:13:11.151Z</v>
+      </c>
+      <c r="B54" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C54" t="str">
+        <v>https://dga.gov.sa</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E54" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F54" t="str">
+        <v>٤:١٣:١١ م</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>2025-12-09T13:14:42.767Z</v>
+      </c>
+      <c r="B55" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C55" t="str">
+        <v>https://dga.gov.sa</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E55" t="str">
+        <v>٩‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F55" t="str">
+        <v>٤:١٤:٤٢ م</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>2025-12-10T06:25:33.109Z</v>
+      </c>
+      <c r="B56" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C56" t="str">
+        <v>https://dga.gov.sa</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E56" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F56" t="str">
+        <v>٩:٢٥:٣٣ ص</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>2025-12-10T06:43:43.388Z</v>
+      </c>
+      <c r="B57" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C57" t="str">
+        <v>https://dga.gov.sa</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E57" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F57" t="str">
+        <v>٩:٤٣:٤٣ ص</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>2025-12-10T07:06:05.108Z</v>
+      </c>
+      <c r="B58" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C58" t="str">
+        <v>https://pnu.edu.sa</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E58" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F58" t="str">
+        <v>١٠:٠٦:٠٥ ص</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>2025-12-10T07:11:56.072Z</v>
+      </c>
+      <c r="B59" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C59" t="str">
+        <v>https://hrdf.org.sa</v>
+      </c>
+      <c r="D59" t="str">
+        <v>No</v>
+      </c>
+      <c r="E59" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F59" t="str">
+        <v>١٠:١١:٥٦ ص</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>2025-12-10T07:18:53.455Z</v>
+      </c>
+      <c r="B60" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C60" t="str">
+        <v>https://hrdf.org.sa</v>
+      </c>
+      <c r="D60" t="str">
+        <v>No</v>
+      </c>
+      <c r="E60" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F60" t="str">
+        <v>١٠:١٨:٥٣ ص</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>2025-12-10T08:14:22.546Z</v>
+      </c>
+      <c r="B61" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C61" t="str">
+        <v>https://hrdf.org.sa</v>
+      </c>
+      <c r="D61" t="str">
+        <v>No</v>
+      </c>
+      <c r="E61" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F61" t="str">
+        <v>١١:١٤:٢٢ ص</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>2025-12-10T08:21:12.958Z</v>
+      </c>
+      <c r="B62" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C62" t="str">
+        <v>https://hrdf.org.sa</v>
+      </c>
+      <c r="D62" t="str">
+        <v>No</v>
+      </c>
+      <c r="E62" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F62" t="str">
+        <v>١١:٢١:١٢ ص</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>2025-12-10T08:42:01.182Z</v>
+      </c>
+      <c r="B63" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C63" t="str">
+        <v>https://pnu.edu.sa</v>
+      </c>
+      <c r="D63" t="str">
+        <v>No</v>
+      </c>
+      <c r="E63" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F63" t="str">
+        <v>١١:٤٢:٠١ ص</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>2025-12-10T08:49:02.598Z</v>
+      </c>
+      <c r="B64" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C64" t="str">
+        <v>https://dga.gov.sa</v>
+      </c>
+      <c r="D64" t="str">
+        <v>No</v>
+      </c>
+      <c r="E64" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F64" t="str">
+        <v>١١:٤٩:٠٢ ص</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>2025-12-10T08:55:39.678Z</v>
+      </c>
+      <c r="B65" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C65" t="str">
+        <v>https://dga.gov.sa</v>
+      </c>
+      <c r="D65" t="str">
+        <v>No</v>
+      </c>
+      <c r="E65" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F65" t="str">
+        <v>١١:٥٥:٣٩ ص</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>2025-12-10T08:58:52.955Z</v>
+      </c>
+      <c r="B66" t="str">
+        <v>rousol@ramworld.net</v>
+      </c>
+      <c r="C66" t="str">
+        <v>https://dga.gov.sa</v>
+      </c>
+      <c r="D66" t="str">
+        <v>No</v>
+      </c>
+      <c r="E66" t="str">
+        <v>١٠‏/١٢‏/٢٠٢٥</v>
+      </c>
+      <c r="F66" t="str">
+        <v>١١:٥٨:٥٢ ص</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F66"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>